<commit_message>
adjust data processing + building summary
</commit_message>
<xml_diff>
--- a/keys/submeter_building_key.xlsx
+++ b/keys/submeter_building_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasm/Dropbox/Dickinson/My courses/2026 Env Data Analysis/dickinson_power/keys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA83DAF2-85F3-564F-AEDE-9BD390AC1EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6C1835-0DAD-354E-BEF5-F8D0C6173801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26420" yWindow="9080" windowWidth="22740" windowHeight="16700" xr2:uid="{69C40327-3D5F-6740-AA56-C48431514492}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>building</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Stern Center</t>
+  </si>
+  <si>
+    <t>Kaufman Hall</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -536,13 +570,13 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -605,11 +639,17 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -671,6 +711,9 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -729,6 +772,22 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$N8=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$L8=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$N9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$L9=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>